<commit_message>
refactor: organizar pipeline em funcoes e adicionar estrutura profissional
</commit_message>
<xml_diff>
--- a/output/relatorio_resumo.xlsx
+++ b/output/relatorio_resumo.xlsx
@@ -8,8 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="Resumo Geral" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Média por Curso" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Taxa Aprovação" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Media por Curso" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Taxa Aprovacao" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Top 5" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>

</xml_diff>